<commit_message>
trip ds-r1 in progress
</commit_message>
<xml_diff>
--- a/output/SMT/DeepSeek-R1/calendar/n_pass/error analysis.xlsx
+++ b/output/SMT/DeepSeek-R1/calendar/n_pass/error analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laiqimei/Desktop/Academic/UPenn/CCB Lab/Project/calendar-planning/output/SMT/DeepSeek-R1/calendar/n_pass/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC8F7A7-A76F-A14A-AC30-EDB1742DDD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A8BD2F-8394-E344-845F-768A6BA53C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="4560" windowWidth="27640" windowHeight="16940" xr2:uid="{9C31B72F-F704-5D48-B5FE-494E628439BF}"/>
+    <workbookView xWindow="3880" yWindow="1480" windowWidth="27640" windowHeight="16940" xr2:uid="{9C31B72F-F704-5D48-B5FE-494E628439BF}"/>
   </bookViews>
   <sheets>
     <sheet name="meeting" sheetId="2" r:id="rId1"/>
@@ -543,7 +543,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1022,7 +1022,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>